<commit_message>
VALIDACIONES DE FORMULARIO LOGIN, INTEGRACION DE DOS PLUGINS PARA ALERTAS, ADAPTACION DE FORMULARIO DE REGISTRO, CONEXION DE PAGINAS REGISTRO-LOGIN
</commit_message>
<xml_diff>
--- a/Trabajos OpinApp.xlsx
+++ b/Trabajos OpinApp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Equipo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gabriel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>CRONOGRAMA DE ACTIVIDADES REALIZADAS</t>
   </si>
@@ -35,25 +35,46 @@
     <t>TAREA</t>
   </si>
   <si>
-    <t>NUEVO DESARROLLO</t>
-  </si>
-  <si>
     <t>ACTUALIZACION</t>
   </si>
   <si>
     <t>RESOLUCION DE BUG</t>
   </si>
   <si>
-    <t>* Adaptación de plantilla AdminLTE para ser usada con Laravel</t>
-  </si>
-  <si>
-    <t>* Login por email y usuario</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>* Carga al servidor de producción</t>
+    <t>NUEVO(a) DESARROLLO / INTEGRACION</t>
+  </si>
+  <si>
+    <t>*Integración maquetado del select pais en el formualario de registro.</t>
+  </si>
+  <si>
+    <t>*Inclusión de plugin sweetalert (para modales y ventanas de confirmación).</t>
+  </si>
+  <si>
+    <t>*Inclusión de plugin ohsnap (para notidicaciones).</t>
+  </si>
+  <si>
+    <t>*Cifrado de clave en SHA-256.</t>
+  </si>
+  <si>
+    <t>*Conexión entre la ventana página registro y login</t>
+  </si>
+  <si>
+    <t>*Conexión entre la ventana página login y registro.</t>
+  </si>
+  <si>
+    <t>* Carga al servidor de producción.</t>
+  </si>
+  <si>
+    <t>* Login por email y usuario.</t>
+  </si>
+  <si>
+    <t>* Adaptación de plantilla AdminLTE para ser usada con Laravel.</t>
+  </si>
+  <si>
+    <t>* Validación de los campos correo y clave en el login</t>
   </si>
 </sst>
 </file>
@@ -98,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -178,16 +199,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -198,32 +267,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -506,90 +605,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>43143</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <v>43143</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>43144</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="18" t="s">
+      <c r="C8" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
+        <v>43145</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A6:A12"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
CREACION DE VENTANA DE ERROR, SELECT CON BUSCADOR EN LA VENTANA REGISTRO
</commit_message>
<xml_diff>
--- a/Trabajos OpinApp.xlsx
+++ b/Trabajos OpinApp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>CRONOGRAMA DE ACTIVIDADES REALIZADAS</t>
   </si>
@@ -74,14 +74,20 @@
     <t>* Adaptación de plantilla AdminLTE para ser usada con Laravel.</t>
   </si>
   <si>
-    <t>* Validación de los campos correo y clave en el login</t>
+    <t>*Maquetación de  ventana de error.</t>
+  </si>
+  <si>
+    <t>*Implementación de un Select con input en el formulario de registro.</t>
+  </si>
+  <si>
+    <t>* Validación de los campos correo y clave en el login.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +110,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -254,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,34 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -325,6 +310,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,29 +618,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="68.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -651,123 +664,134 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="23">
         <v>43143</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="23">
         <v>43144</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="11">
         <v>43145</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
FILTRO VOTOS, FECHA, BUSCADOR
</commit_message>
<xml_diff>
--- a/Trabajos OpinApp.xlsx
+++ b/Trabajos OpinApp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>FECHA</t>
   </si>
@@ -291,6 +291,83 @@
   <si>
     <t>Resolucion de duda  a cerca de la consulta para Top Usuarios con el amigo gabriel</t>
   </si>
+  <si>
+    <t>Descarga e instalación de software para la sincronización de carpetas.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nº Actividades</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 25 | </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Horas trabajadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 10 |</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Monto Facturado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">50 USD </t>
+    </r>
+  </si>
+  <si>
+    <t>Retiro de fecha duplicada en Opin más votados</t>
+  </si>
+  <si>
+    <t>Listado de opins publicos con funcion Ajax</t>
+  </si>
+  <si>
+    <t>Imagen de usuario dinamica en el header y el aside</t>
+  </si>
 </sst>
 </file>
 
@@ -326,8 +403,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -488,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -550,8 +627,11 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,13 +997,13 @@
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -947,38 +1027,38 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
+      <c r="A7" s="36">
         <v>43143</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="43"/>
+      <c r="C7" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="44"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="44"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="44"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -989,7 +1069,7 @@
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
+      <c r="A11" s="36">
         <v>43144</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1002,7 +1082,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1093,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
@@ -1024,7 +1104,7 @@
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="8" t="s">
         <v>46</v>
       </c>
@@ -1033,7 +1113,7 @@
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
@@ -1044,7 +1124,7 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="8" t="s">
         <v>45</v>
       </c>
@@ -1053,7 +1133,7 @@
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="8"/>
       <c r="C17" s="18" t="s">
         <v>4</v>
@@ -1062,7 +1142,7 @@
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="35">
+      <c r="A18" s="36">
         <v>43145</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -1075,7 +1155,7 @@
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="19" t="s">
         <v>43</v>
       </c>
@@ -1086,7 +1166,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="19" t="s">
         <v>42</v>
       </c>
@@ -1097,7 +1177,7 @@
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
@@ -1108,7 +1188,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
@@ -1119,7 +1199,7 @@
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="35">
+      <c r="A23" s="36">
         <v>43146</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1132,7 +1212,7 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="17" t="s">
         <v>19</v>
       </c>
@@ -1143,7 +1223,7 @@
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="17" t="s">
         <v>40</v>
       </c>
@@ -1154,7 +1234,7 @@
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="17" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1245,7 @@
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
@@ -1176,7 +1256,7 @@
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="17" t="s">
         <v>20</v>
       </c>
@@ -1187,7 +1267,7 @@
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="17" t="s">
         <v>23</v>
       </c>
@@ -1198,7 +1278,7 @@
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="35">
+      <c r="A30" s="36">
         <v>43147</v>
       </c>
       <c r="B30" s="26" t="s">
@@ -1211,7 +1291,7 @@
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="17" t="s">
         <v>21</v>
       </c>
@@ -1222,7 +1302,7 @@
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="17" t="s">
         <v>24</v>
       </c>
@@ -1233,7 +1313,7 @@
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="17" t="s">
         <v>38</v>
       </c>
@@ -1244,7 +1324,7 @@
       <c r="E33" s="13"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="17" t="s">
         <v>37</v>
       </c>
@@ -1255,7 +1335,7 @@
       <c r="E34" s="13"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="27" t="s">
         <v>36</v>
       </c>
@@ -1266,7 +1346,7 @@
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="17" t="s">
         <v>35</v>
       </c>
@@ -1277,7 +1357,7 @@
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="17" t="s">
         <v>9</v>
       </c>
@@ -1288,7 +1368,7 @@
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="19" t="s">
         <v>34</v>
       </c>
@@ -1299,7 +1379,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="20" t="s">
         <v>33</v>
       </c>
@@ -1327,7 +1407,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="35">
+      <c r="A42" s="36">
         <v>43151</v>
       </c>
       <c r="B42" s="31" t="s">
@@ -1335,124 +1415,174 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
+      <c r="A43" s="37"/>
       <c r="B43" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="36"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="36"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="30" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="30" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="35">
+      <c r="A48" s="36">
         <v>43152</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
-      <c r="B49" s="34" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="37"/>
+      <c r="B49" s="33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="36"/>
-      <c r="B50" s="34" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="37"/>
+      <c r="B50" s="33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="34" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="37"/>
+      <c r="B51" s="33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="36"/>
-      <c r="B52" s="34" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="37"/>
+      <c r="B52" s="33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="36"/>
-      <c r="B53" s="34" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="37"/>
+      <c r="B53" s="33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="36"/>
-      <c r="B54" s="34" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="37"/>
+      <c r="B54" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="36"/>
-      <c r="B55" s="34" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="37"/>
+      <c r="B55" s="33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="37"/>
-      <c r="B56" s="34" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="38"/>
+      <c r="B56" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="32">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="36">
         <v>43153</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="37"/>
       <c r="B58" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="37"/>
       <c r="B59" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="37"/>
       <c r="B60" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="38"/>
       <c r="B61" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="33"/>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="36">
+        <v>43154</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="37"/>
+      <c r="B63" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+    </row>
+    <row r="64" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="37"/>
+      <c r="B64" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+    </row>
+    <row r="65" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="38"/>
+      <c r="B65" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+    </row>
+    <row r="66" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A48:A56"/>
     <mergeCell ref="A42:A47"/>
     <mergeCell ref="A30:A39"/>
     <mergeCell ref="A5:E5"/>
@@ -1463,7 +1593,6 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="A23:A29"/>
-    <mergeCell ref="A48:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CONFIGURACION CON SERVIDOR DE PRODUCCION
</commit_message>
<xml_diff>
--- a/Trabajos OpinApp.xlsx
+++ b/Trabajos OpinApp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>FECHA</t>
   </si>
@@ -295,6 +295,66 @@
     <t>Descarga e instalación de software para la sincronización de carpetas.</t>
   </si>
   <si>
+    <t>Retiro de fecha duplicada en Opin más votados</t>
+  </si>
+  <si>
+    <t>Listado de opins publicos con funcion Ajax</t>
+  </si>
+  <si>
+    <t>Imagen de usuario dinamica en el header y el aside</t>
+  </si>
+  <si>
+    <t>Filtro de buscador haciendo uso de funcion ajax()</t>
+  </si>
+  <si>
+    <t>Fitro votos: Organizar de manera asc y desc haciendo uso de funcion ajax()</t>
+  </si>
+  <si>
+    <t>Filtro fecha:  Organizar de manera asc y desc haciendo uso de funcion ajax()</t>
+  </si>
+  <si>
+    <t>Filtro: Categoría</t>
+  </si>
+  <si>
+    <t>Completar el menú de settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quitar el menu inicio del aside </t>
+  </si>
+  <si>
+    <t>Crear perfil de super su</t>
+  </si>
+  <si>
+    <t>Mostrar si el opin es publico</t>
+  </si>
+  <si>
+    <t>Mostrar si el opin puede ser votado solo una vez</t>
+  </si>
+  <si>
+    <t>Saber si tiene fecha final</t>
+  </si>
+  <si>
+    <t>Crearvista en la base de datos con toda la informacion relacionada a las encuestas</t>
+  </si>
+  <si>
+    <t>Cambio de texto publico por iconos</t>
+  </si>
+  <si>
+    <t>Cambio de texto seleccion unica por icono</t>
+  </si>
+  <si>
+    <t>Colocacion de banderas a las fecha de publicacion y finalizacion de los opins</t>
+  </si>
+  <si>
+    <t>Maquetacion de vista para opins no votados.</t>
+  </si>
+  <si>
+    <t>Cambio de color de corazon si el usuario ya le ha seleccionado ese opins como favorito</t>
+  </si>
+  <si>
+    <t>Creacion de vista de encuesta total con asistencia del estimado Gabriel.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -314,7 +374,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 25 | </t>
+      <t xml:space="preserve"> 30 | </t>
     </r>
     <r>
       <rPr>
@@ -360,58 +420,55 @@
     </r>
   </si>
   <si>
-    <t>Retiro de fecha duplicada en Opin más votados</t>
-  </si>
-  <si>
-    <t>Listado de opins publicos con funcion Ajax</t>
-  </si>
-  <si>
-    <t>Imagen de usuario dinamica en el header y el aside</t>
-  </si>
-  <si>
-    <t>Filtro de buscador haciendo uso de funcion ajax()</t>
-  </si>
-  <si>
-    <t>Fitro votos: Organizar de manera asc y desc haciendo uso de funcion ajax()</t>
-  </si>
-  <si>
-    <t>Filtro fecha:  Organizar de manera asc y desc haciendo uso de funcion ajax()</t>
-  </si>
-  <si>
-    <t>Filtro: Categoría</t>
-  </si>
-  <si>
-    <t>Crear login con facebook</t>
-  </si>
-  <si>
-    <t>Crear login con twiter</t>
-  </si>
-  <si>
-    <t>Colocarle las flechas a los botones</t>
-  </si>
-  <si>
-    <t>Completar el menú de settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quitar el menu inicio del aside </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Crear perfil de super su</t>
-  </si>
-  <si>
-    <t>Mostrar si el opin es publico</t>
-  </si>
-  <si>
-    <t>Mostrar si el opin puede ser votado solo una vez</t>
-  </si>
-  <si>
-    <t>Saber si tiene fecha final</t>
-  </si>
-  <si>
-    <t>Colocar contador si tiene fecha final</t>
+    <t>Cambiar el icono de publico</t>
+  </si>
+  <si>
+    <t>Cambiar de lugar la fecha de finalización</t>
+  </si>
+  <si>
+    <t>Cambio de consulta para filtrar por fechaInicio y no por fecha creacion</t>
+  </si>
+  <si>
+    <t>Instalacion de software para la sincronización de carpetas entre el estimado gabriel y mi persona.</t>
+  </si>
+  <si>
+    <t>Cambiar el color del icono favorito si el usuario lo ha seleccionado como favorito.</t>
+  </si>
+  <si>
+    <t>Colocar icono de banderas a las fechas (opins mas votados)</t>
+  </si>
+  <si>
+    <t>Colocar fecha de finalización (opins mas votados)</t>
+  </si>
+  <si>
+    <t>Colocar icono de solo puede ser votado una vez(opins mas votados)</t>
+  </si>
+  <si>
+    <t>Colocar icono de estado publico o privado (opins mas votados)</t>
+  </si>
+  <si>
+    <t>Maquetacion de la vista de perfil de usuario</t>
+  </si>
+  <si>
+    <t>Creacción de app de prueba en facebook</t>
+  </si>
+  <si>
+    <t>Estudio de SDK de facebook</t>
+  </si>
+  <si>
+    <t>Adaptacion de codigo js para usar el SDK de facebook</t>
+  </si>
+  <si>
+    <t>Login de prueba en html y js con la app de prueba creada en facebook haciendo uso del SDK</t>
+  </si>
+  <si>
+    <t>Resolver problema de referencias en el servidor.</t>
+  </si>
+  <si>
+    <t>Establecer conexión con el servidor FTP</t>
+  </si>
+  <si>
+    <t>Actualizacion de controladores para que funcione en el servidor (Problema de mayusculas en las tablas)</t>
   </si>
 </sst>
 </file>
@@ -625,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -695,8 +752,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,26 +783,14 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,13 +1127,13 @@
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1092,38 +1157,38 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="45">
         <v>43143</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="47"/>
+      <c r="C7" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="48"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="48"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="44"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1134,7 +1199,7 @@
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="45">
         <v>43144</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1147,7 +1212,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
@@ -1158,7 +1223,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
@@ -1169,7 +1234,7 @@
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="8" t="s">
         <v>46</v>
       </c>
@@ -1178,7 +1243,7 @@
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
@@ -1189,7 +1254,7 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="8" t="s">
         <v>45</v>
       </c>
@@ -1198,7 +1263,7 @@
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="8"/>
       <c r="C17" s="18" t="s">
         <v>4</v>
@@ -1207,7 +1272,7 @@
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="45">
         <v>43145</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -1220,7 +1285,7 @@
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="19" t="s">
         <v>43</v>
       </c>
@@ -1231,7 +1296,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="19" t="s">
         <v>42</v>
       </c>
@@ -1242,7 +1307,7 @@
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1318,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
@@ -1264,7 +1329,7 @@
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+      <c r="A23" s="45">
         <v>43146</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1277,7 +1342,7 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="17" t="s">
         <v>19</v>
       </c>
@@ -1288,7 +1353,7 @@
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="17" t="s">
         <v>40</v>
       </c>
@@ -1299,7 +1364,7 @@
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="17" t="s">
         <v>7</v>
       </c>
@@ -1310,7 +1375,7 @@
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
@@ -1321,7 +1386,7 @@
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="17" t="s">
         <v>20</v>
       </c>
@@ -1332,7 +1397,7 @@
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="17" t="s">
         <v>23</v>
       </c>
@@ -1343,7 +1408,7 @@
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="39">
+      <c r="A30" s="45">
         <v>43147</v>
       </c>
       <c r="B30" s="26" t="s">
@@ -1356,7 +1421,7 @@
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="17" t="s">
         <v>21</v>
       </c>
@@ -1367,7 +1432,7 @@
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="17" t="s">
         <v>24</v>
       </c>
@@ -1378,7 +1443,7 @@
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="17" t="s">
         <v>38</v>
       </c>
@@ -1389,7 +1454,7 @@
       <c r="E33" s="13"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
+      <c r="A34" s="46"/>
       <c r="B34" s="17" t="s">
         <v>37</v>
       </c>
@@ -1400,7 +1465,7 @@
       <c r="E34" s="13"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="27" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1476,7 @@
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
+      <c r="A36" s="46"/>
       <c r="B36" s="17" t="s">
         <v>35</v>
       </c>
@@ -1422,7 +1487,7 @@
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="17" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1498,7 @@
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="19" t="s">
         <v>34</v>
       </c>
@@ -1444,7 +1509,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="20" t="s">
         <v>33</v>
       </c>
@@ -1472,7 +1537,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="39">
+      <c r="A42" s="45">
         <v>43151</v>
       </c>
       <c r="B42" s="31" t="s">
@@ -1480,37 +1545,37 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="40"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
+      <c r="A45" s="46"/>
       <c r="B45" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
+      <c r="A46" s="46"/>
       <c r="B46" s="30" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="41"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="30" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="39">
+      <c r="A48" s="45">
         <v>43152</v>
       </c>
       <c r="B48" s="30" t="s">
@@ -1518,55 +1583,55 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
+      <c r="A49" s="46"/>
       <c r="B49" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="40"/>
+      <c r="A50" s="46"/>
       <c r="B50" s="33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="40"/>
+      <c r="A51" s="46"/>
       <c r="B51" s="33" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="46"/>
       <c r="B52" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="40"/>
+      <c r="A53" s="46"/>
       <c r="B53" s="33" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="40"/>
+      <c r="A54" s="46"/>
       <c r="B54" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="33" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="41"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="33" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="39">
+      <c r="A57" s="45">
         <v>43153</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1574,31 +1639,31 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="40"/>
+      <c r="A58" s="46"/>
       <c r="B58" s="30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="40"/>
+      <c r="A59" s="46"/>
       <c r="B59" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="40"/>
+      <c r="A60" s="46"/>
       <c r="B60" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="39">
+      <c r="A62" s="45">
         <v>43154</v>
       </c>
       <c r="B62" s="30" t="s">
@@ -1606,27 +1671,27 @@
       </c>
     </row>
     <row r="63" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="40"/>
+      <c r="A63" s="46"/>
       <c r="B63" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63" s="34"/>
       <c r="D63" s="34"/>
       <c r="E63" s="34"/>
     </row>
     <row r="64" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
+      <c r="A64" s="46"/>
       <c r="B64" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64" s="34"/>
       <c r="D64" s="34"/>
       <c r="E64" s="34"/>
     </row>
     <row r="65" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="41"/>
+      <c r="A65" s="47"/>
       <c r="B65" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65" s="34"/>
       <c r="D65" s="34"/>
@@ -1637,126 +1702,255 @@
         <v>28</v>
       </c>
       <c r="B66" s="29" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C66" s="28"/>
       <c r="D66" s="28"/>
       <c r="E66" s="28"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="39">
+      <c r="A67" s="45">
         <v>43157</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="46"/>
+      <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="40"/>
-      <c r="B68" s="1" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="46"/>
+      <c r="B69" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="40"/>
-      <c r="B69" s="1" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="47"/>
+      <c r="B70" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="41"/>
-      <c r="B70" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="36"/>
+    <row r="71" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="48">
+        <v>43158</v>
+      </c>
       <c r="B71" s="30" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C71" s="36"/>
       <c r="D71" s="36"/>
       <c r="E71" s="36"/>
     </row>
-    <row r="72" spans="1:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="36"/>
-      <c r="B72" s="37" t="s">
-        <v>79</v>
+    <row r="72" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="49"/>
+      <c r="B72" s="30" t="s">
+        <v>76</v>
       </c>
       <c r="C72" s="36"/>
       <c r="D72" s="36"/>
       <c r="E72" s="36"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="49"/>
       <c r="B73" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="49"/>
+      <c r="B74" s="30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="49"/>
+      <c r="B75" s="30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="30" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="50"/>
+      <c r="B76" s="30" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="30" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="45">
+        <v>43159</v>
+      </c>
+      <c r="B77" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="46"/>
+      <c r="B78" s="30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="46"/>
+      <c r="B79" s="35" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="30" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="46"/>
+      <c r="B80" s="30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="30" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="47"/>
+      <c r="B81" s="30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="45">
+        <v>43160</v>
+      </c>
+      <c r="B82" s="30" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="38" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="37"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="37"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="37"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="37" t="s">
-        <v>82</v>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="46"/>
+      <c r="B83" s="30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="46"/>
+      <c r="B84" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="47"/>
+      <c r="B85" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="45">
+        <v>43161</v>
+      </c>
+      <c r="B86" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="46"/>
+      <c r="B87" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="46"/>
+      <c r="B88" s="30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="46"/>
+      <c r="B89" s="30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="46"/>
+      <c r="B90" s="30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="46"/>
+      <c r="B91" s="30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="46"/>
+      <c r="B92" s="30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="47"/>
+      <c r="B93" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="45">
+        <v>43164</v>
+      </c>
+      <c r="B94" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="46"/>
+      <c r="B95" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="46"/>
+      <c r="B96" s="30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="47"/>
+      <c r="B97" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="32">
+        <v>43165</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="19">
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="A86:A93"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="A71:A76"/>
     <mergeCell ref="A67:A70"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="A23:A29"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A48:A56"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="A82:A85"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A48:A56"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="A30:A39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fix login en produccion
</commit_message>
<xml_diff>
--- a/Trabajos OpinApp.xlsx
+++ b/Trabajos OpinApp.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="137">
   <si>
     <t>FECHA</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>Carga de archivos al servidor de producción</t>
+  </si>
+  <si>
+    <t>Fix de bug por tokken en inicio de sesion</t>
   </si>
 </sst>
 </file>
@@ -858,12 +861,30 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -884,24 +905,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1188,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,13 +1246,13 @@
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1279,32 +1282,32 @@
       <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="51"/>
+      <c r="C7" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="57"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="58"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="58"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1328,7 +1331,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
@@ -1339,7 +1342,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
@@ -1350,7 +1353,7 @@
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="8" t="s">
         <v>46</v>
       </c>
@@ -1359,7 +1362,7 @@
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
@@ -1370,7 +1373,7 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="8" t="s">
         <v>45</v>
       </c>
@@ -1379,7 +1382,7 @@
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="8"/>
       <c r="C17" s="18" t="s">
         <v>4</v>
@@ -1401,7 +1404,7 @@
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="19" t="s">
         <v>43</v>
       </c>
@@ -1412,7 +1415,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="19" t="s">
         <v>42</v>
       </c>
@@ -1423,7 +1426,7 @@
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
@@ -1434,7 +1437,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
@@ -1458,7 +1461,7 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="17" t="s">
         <v>19</v>
       </c>
@@ -1469,7 +1472,7 @@
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="17" t="s">
         <v>40</v>
       </c>
@@ -1480,7 +1483,7 @@
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="17" t="s">
         <v>7</v>
       </c>
@@ -1491,7 +1494,7 @@
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
@@ -1502,7 +1505,7 @@
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="17" t="s">
         <v>20</v>
       </c>
@@ -1513,7 +1516,7 @@
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="45"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="17" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1540,7 @@
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="17" t="s">
         <v>21</v>
       </c>
@@ -1548,7 +1551,7 @@
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="17" t="s">
         <v>24</v>
       </c>
@@ -1559,7 +1562,7 @@
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="17" t="s">
         <v>38</v>
       </c>
@@ -1570,7 +1573,7 @@
       <c r="E33" s="13"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
+      <c r="A34" s="46"/>
       <c r="B34" s="17" t="s">
         <v>37</v>
       </c>
@@ -1581,7 +1584,7 @@
       <c r="E34" s="13"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="27" t="s">
         <v>36</v>
       </c>
@@ -1592,7 +1595,7 @@
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
+      <c r="A36" s="46"/>
       <c r="B36" s="17" t="s">
         <v>35</v>
       </c>
@@ -1603,7 +1606,7 @@
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="17" t="s">
         <v>9</v>
       </c>
@@ -1614,7 +1617,7 @@
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="19" t="s">
         <v>34</v>
       </c>
@@ -1625,7 +1628,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="45"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="20" t="s">
         <v>33</v>
       </c>
@@ -1661,31 +1664,31 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
+      <c r="A45" s="46"/>
       <c r="B45" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
+      <c r="A46" s="46"/>
       <c r="B46" s="30" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="45"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="30" t="s">
         <v>63</v>
       </c>
@@ -1699,49 +1702,49 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
+      <c r="A49" s="46"/>
       <c r="B49" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
+      <c r="A50" s="46"/>
       <c r="B50" s="33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
+      <c r="A51" s="46"/>
       <c r="B51" s="33" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
+      <c r="A52" s="46"/>
       <c r="B52" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="44"/>
+      <c r="A53" s="46"/>
       <c r="B53" s="33" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
+      <c r="A54" s="46"/>
       <c r="B54" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="33" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="33" t="s">
         <v>67</v>
       </c>
@@ -1755,25 +1758,25 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
+      <c r="A58" s="46"/>
       <c r="B58" s="30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
+      <c r="A59" s="46"/>
       <c r="B59" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
+      <c r="A60" s="46"/>
       <c r="B60" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="45"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="1" t="s">
         <v>53</v>
       </c>
@@ -1787,7 +1790,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
+      <c r="A63" s="46"/>
       <c r="B63" s="30" t="s">
         <v>71</v>
       </c>
@@ -1796,7 +1799,7 @@
       <c r="E63" s="34"/>
     </row>
     <row r="64" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
+      <c r="A64" s="46"/>
       <c r="B64" s="30" t="s">
         <v>69</v>
       </c>
@@ -1805,7 +1808,7 @@
       <c r="E64" s="34"/>
     </row>
     <row r="65" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="45"/>
+      <c r="A65" s="47"/>
       <c r="B65" s="30" t="s">
         <v>70</v>
       </c>
@@ -1833,25 +1836,25 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
+      <c r="A68" s="46"/>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
+      <c r="A69" s="46"/>
       <c r="B69" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="45"/>
+      <c r="A70" s="47"/>
       <c r="B70" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="55">
+      <c r="A71" s="48">
         <v>43158</v>
       </c>
       <c r="B71" s="30" t="s">
@@ -1862,7 +1865,7 @@
       <c r="E71" s="36"/>
     </row>
     <row r="72" spans="1:5" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="56"/>
+      <c r="A72" s="49"/>
       <c r="B72" s="30" t="s">
         <v>76</v>
       </c>
@@ -1871,25 +1874,25 @@
       <c r="E72" s="36"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="56"/>
+      <c r="A73" s="49"/>
       <c r="B73" s="30" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="56"/>
+      <c r="A74" s="49"/>
       <c r="B74" s="30" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="56"/>
+      <c r="A75" s="49"/>
       <c r="B75" s="30" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="57"/>
+      <c r="A76" s="50"/>
       <c r="B76" s="30" t="s">
         <v>81</v>
       </c>
@@ -1903,25 +1906,25 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="44"/>
+      <c r="A78" s="46"/>
       <c r="B78" s="30" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="44"/>
+      <c r="A79" s="46"/>
       <c r="B79" s="35" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
+      <c r="A80" s="46"/>
       <c r="B80" s="30" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="45"/>
+      <c r="A81" s="47"/>
       <c r="B81" s="30" t="s">
         <v>87</v>
       </c>
@@ -1935,19 +1938,19 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="44"/>
+      <c r="A83" s="46"/>
       <c r="B83" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
+      <c r="A84" s="46"/>
       <c r="B84" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="45"/>
+      <c r="A85" s="47"/>
       <c r="B85" s="1" t="s">
         <v>93</v>
       </c>
@@ -1961,43 +1964,43 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="44"/>
+      <c r="A87" s="46"/>
       <c r="B87" s="30" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="44"/>
+      <c r="A88" s="46"/>
       <c r="B88" s="30" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="44"/>
+      <c r="A89" s="46"/>
       <c r="B89" s="30" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="44"/>
+      <c r="A90" s="46"/>
       <c r="B90" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="44"/>
+      <c r="A91" s="46"/>
       <c r="B91" s="30" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="44"/>
+      <c r="A92" s="46"/>
       <c r="B92" s="30" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="45"/>
+      <c r="A93" s="47"/>
       <c r="B93" s="30" t="s">
         <v>99</v>
       </c>
@@ -2011,19 +2014,19 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="44"/>
+      <c r="A95" s="46"/>
       <c r="B95" s="30" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="44"/>
+      <c r="A96" s="46"/>
       <c r="B96" s="30" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="45"/>
+      <c r="A97" s="47"/>
       <c r="B97" s="30" t="s">
         <v>103</v>
       </c>
@@ -2037,31 +2040,31 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="44"/>
+      <c r="A99" s="46"/>
       <c r="B99" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
+      <c r="A100" s="46"/>
       <c r="B100" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
+      <c r="A101" s="46"/>
       <c r="B101" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="45"/>
+      <c r="A102" s="47"/>
       <c r="B102" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="58" t="s">
+      <c r="A103" s="51" t="s">
         <v>109</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -2069,37 +2072,37 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="53"/>
+      <c r="A104" s="44"/>
       <c r="B104" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="53"/>
+      <c r="A105" s="44"/>
       <c r="B105" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="53"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="30" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="53"/>
+      <c r="A107" s="44"/>
       <c r="B107" s="30" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="53"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="30" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="54"/>
+      <c r="A109" s="45"/>
       <c r="B109" s="30" t="s">
         <v>119</v>
       </c>
@@ -2113,19 +2116,19 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="44"/>
+      <c r="A111" s="46"/>
       <c r="B111" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="44"/>
+      <c r="A112" s="46"/>
       <c r="B112" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="45"/>
+      <c r="A113" s="47"/>
       <c r="B113" s="30" t="s">
         <v>118</v>
       </c>
@@ -2139,43 +2142,43 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="53"/>
+      <c r="A115" s="44"/>
       <c r="B115" s="38" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="53"/>
+      <c r="A116" s="44"/>
       <c r="B116" s="38" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="53"/>
+      <c r="A117" s="44"/>
       <c r="B117" s="38" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="53"/>
+      <c r="A118" s="44"/>
       <c r="B118" s="33" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="53"/>
+      <c r="A119" s="44"/>
       <c r="B119" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="53"/>
+      <c r="A120" s="44"/>
       <c r="B120" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="54"/>
+      <c r="A121" s="45"/>
       <c r="B121" s="1" t="s">
         <v>127</v>
       </c>
@@ -2222,13 +2225,28 @@
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
         <v>135</v>
       </c>
     </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="32">
+        <v>43173</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="A86:A93"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="A7:A10"/>
     <mergeCell ref="A114:A121"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A18:A22"/>
@@ -2245,13 +2263,6 @@
     <mergeCell ref="A82:A85"/>
     <mergeCell ref="A103:A109"/>
     <mergeCell ref="A98:A102"/>
-    <mergeCell ref="A94:A97"/>
-    <mergeCell ref="A86:A93"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A7:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>